<commit_message>
Partial resolution of plotting
</commit_message>
<xml_diff>
--- a/11-Parameters/LIONBeamLine-Params-Gauss.xlsx
+++ b/11-Parameters/LIONBeamLine-Params-Gauss.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A718AD-59D4-A24E-ACE3-13E64D7E4220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B10866-AF49-DA4C-8DB2-E7E2BD3F3A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="27880" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="60">
   <si>
     <t>Parameter</t>
   </si>
@@ -711,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A20" sqref="A20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,20 +1085,22 @@
         <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E15" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F15" s="3">
-        <v>0.04</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1113,16 +1115,16 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F16" s="3">
-        <v>332</v>
+        <v>0.04</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1133,22 +1135,20 @@
         <v>23</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F17" s="3">
-        <v>5.0000000000000001E-3</v>
+        <v>332</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1159,20 +1159,22 @@
         <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E18" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F18" s="3">
-        <v>3.6953E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1183,20 +1185,20 @@
         <v>23</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="3">
-        <v>0.02</v>
+        <v>3.6953E-2</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1207,46 +1209,46 @@
         <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="3">
-        <v>318.5</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>1</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>37</v>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1254,47 +1256,49 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F22" s="3">
-        <v>1.6</v>
+        <v>318.5</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>40</v>
+      <c r="A23" s="4">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1305,45 +1309,93 @@
         <v>38</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F26" s="3">
         <v>1.5E-3</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="G26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>1</v>
-      </c>
-      <c r="B25" s="4" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4" t="s">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F27" s="4">
         <v>0.02</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="4" t="s">
+      <c r="G27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add uniform disc source
</commit_message>
<xml_diff>
--- a/11-Parameters/LIONBeamLine-Params-Gauss.xlsx
+++ b/11-Parameters/LIONBeamLine-Params-Gauss.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B10866-AF49-DA4C-8DB2-E7E2BD3F3A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8828650A-7173-8E45-9551-DAF1926EE023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="27880" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="61">
   <si>
     <t>Parameter</t>
   </si>
@@ -173,9 +173,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Parameterised TNSA</t>
-  </si>
-  <si>
     <t>Facility</t>
   </si>
   <si>
@@ -216,6 +213,12 @@
   </si>
   <si>
     <t>Minimum theta for flat cos theta</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Gaussian</t>
   </si>
 </sst>
 </file>
@@ -714,7 +717,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:H20"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,19 +763,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -782,16 +785,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="D3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>51</v>
       </c>
       <c r="F3" s="11">
         <v>10</v>
@@ -806,16 +809,16 @@
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="D4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="F4" s="8">
         <v>0.5</v>
@@ -836,7 +839,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
@@ -846,7 +849,7 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -860,7 +863,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
@@ -886,7 +889,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
@@ -912,10 +915,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" s="2">
         <v>10</v>
@@ -924,7 +927,7 @@
         <v>9</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -938,10 +941,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="2">
         <v>0.3</v>
@@ -950,7 +953,7 @@
         <v>9</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -964,7 +967,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>18</v>
@@ -974,7 +977,7 @@
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1202,8 +1205,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>1</v>
+      <c r="A20" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>23</v>

</xml_diff>